<commit_message>
Update ORGANIZAÇÃO DE DECLARAÇÃO DE IMPOSTO DE RENDA.xlsx
</commit_message>
<xml_diff>
--- a/ORGANIZAÇÃO DE DECLARAÇÃO DE IMPOSTO DE RENDA.xlsx
+++ b/ORGANIZAÇÃO DE DECLARAÇÃO DE IMPOSTO DE RENDA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruna\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruna\Documents\declaração\Organizador-de-Declaracao-de-Imposto-de-Renda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5428D121-A805-49E7-A81F-653AE63D7977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F36F230-5C8D-41F1-8B70-29886F3C11EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="399" activeTab="2" xr2:uid="{FE444B7E-C467-4AA8-97D8-A573C3E12BDD}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
   <si>
     <t>NOME</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>FREELANCE</t>
+  </si>
+  <si>
+    <t>BRUNA PEDROSA GUEDES</t>
   </si>
 </sst>
 </file>
@@ -332,11 +335,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="168" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
-    <numFmt numFmtId="170" formatCode="00000\-000"/>
-    <numFmt numFmtId="171" formatCode="&quot;(&quot;00&quot;)&quot;0000&quot;-&quot;0000"/>
-    <numFmt numFmtId="172" formatCode="&quot;(&quot;00&quot;)&quot;00000&quot;-&quot;0000"/>
-    <numFmt numFmtId="173" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
+    <numFmt numFmtId="165" formatCode="00000\-000"/>
+    <numFmt numFmtId="166" formatCode="&quot;(&quot;00&quot;)&quot;0000&quot;-&quot;0000"/>
+    <numFmt numFmtId="167" formatCode="&quot;(&quot;00&quot;)&quot;00000&quot;-&quot;0000"/>
+    <numFmt numFmtId="168" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -515,7 +518,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -527,33 +530,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -566,19 +556,19 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -586,7 +576,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -598,9 +588,21 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -611,16 +613,16 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="173" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <numFmt numFmtId="168" formatCode="&quot;R$&quot;\ #,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="168" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="173" formatCode="&quot;R$&quot;\ #,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -971,6 +973,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3310-43EF-B2F1-5A253BE89DFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -986,6 +993,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3310-43EF-B2F1-5A253BE89DFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1001,6 +1013,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-3310-43EF-B2F1-5A253BE89DFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1016,6 +1033,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3310-43EF-B2F1-5A253BE89DFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -4518,12 +4540,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9851D9E6-38D7-4EE0-A570-90F2998AD03C}" name="Tabela2" displayName="Tabela2" ref="C7:E24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9851D9E6-38D7-4EE0-A570-90F2998AD03C}" name="Tabela2" displayName="Tabela2" ref="C7:E24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="C7:E24" xr:uid="{9851D9E6-38D7-4EE0-A570-90F2998AD03C}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D6ED5272-B37F-4678-B14D-E04FDB25C323}" name="DATA" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4489A6E7-30A9-45A2-860F-F9A8A5CACE52}" name="CATEGORIA" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{221B4640-0F8A-4818-80C3-2106137396DD}" name="VALOR" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{D6ED5272-B37F-4678-B14D-E04FDB25C323}" name="DATA" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4489A6E7-30A9-45A2-860F-F9A8A5CACE52}" name="CATEGORIA" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{221B4640-0F8A-4818-80C3-2106137396DD}" name="VALOR" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4861,7 +4883,7 @@
   <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4878,11 +4900,11 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="3:8" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H4" s="6"/>
@@ -4891,15 +4913,15 @@
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>16</v>
+      <c r="D5" s="15" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="16">
         <v>4685468468</v>
       </c>
     </row>
@@ -4907,7 +4929,7 @@
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4915,7 +4937,7 @@
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="15">
         <v>585868686</v>
       </c>
     </row>
@@ -4923,7 +4945,7 @@
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4931,7 +4953,7 @@
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="15" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4939,7 +4961,7 @@
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4947,7 +4969,7 @@
       <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="17">
         <v>543654654</v>
       </c>
     </row>
@@ -4955,7 +4977,7 @@
       <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="18">
         <v>4635463543</v>
       </c>
     </row>
@@ -4963,7 +4985,7 @@
       <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="19">
         <v>54635465</v>
       </c>
     </row>
@@ -4971,7 +4993,7 @@
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4979,7 +5001,7 @@
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4987,7 +5009,7 @@
       <c r="C17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4995,7 +5017,7 @@
       <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5038,163 +5060,154 @@
     <col min="3" max="4" width="46.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="9" t="s">
+    <row r="2" spans="3:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+    <row r="3" spans="3:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="14">
+    <row r="6" spans="3:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="27">
         <f>SUM(D10+D15+D20+D25)</f>
         <v>72000</v>
       </c>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="12" t="s">
+      <c r="D6" s="28"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="21">
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="C12" s="13"/>
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="12" t="s">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="21">
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="C17" s="13"/>
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="12" t="s">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="21">
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="C22" s="13"/>
-      <c r="D22"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="12" t="s">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="21">
         <v>30000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5241,129 +5254,129 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="3:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="16"/>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="16"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="27">
+      <c r="C8" s="22">
         <v>45831</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="24">
         <v>3000</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="28"/>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="23"/>
+      <c r="D10" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -5412,7 +5425,7 @@
         <f>INFORMES!D9</f>
         <v>77 - Banco Inter</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="12">
         <f>INFORMES!D10</f>
         <v>10000</v>
       </c>
@@ -5422,7 +5435,7 @@
         <f>INFORMES!D14</f>
         <v>33 - Banco Santander</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="12">
         <f>INFORMES!D15</f>
         <v>2000</v>
       </c>
@@ -5432,7 +5445,7 @@
         <f>INFORMES!D19</f>
         <v>33 - Banco Santander</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="12">
         <f>INFORMES!D20</f>
         <v>30000</v>
       </c>
@@ -5442,7 +5455,7 @@
         <f>INFORMES!D24</f>
         <v>341 - Itaú Unibanco</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="12">
         <f>INFORMES!D25</f>
         <v>30000</v>
       </c>
@@ -5470,257 +5483,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="A32" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="A33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="A34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="A36" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="A37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+      <c r="A38" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="A39" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+      <c r="A40" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="A42" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="A43" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+      <c r="A44" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+      <c r="A45" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
+      <c r="A46" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+      <c r="A47" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+      <c r="A48" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+      <c r="A49" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+      <c r="A50" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="A51" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>